<commit_message>
adding most up to date data input files
</commit_message>
<xml_diff>
--- a/data/case study data copy.xlsx
+++ b/data/case study data copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnryter/Dropbox (MIT)/John MIT/Research/generalizationOutside/generalization/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBC357C-6306-0042-8EAD-9F57F6B21EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E2435C-66E9-E047-8044-6CB1CCAF32F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{9C1DBEC5-9C42-494B-AEAA-1D89B674AD0D}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="375">
   <si>
     <t>Al</t>
   </si>
@@ -874,12 +874,6 @@
     <t>https://tantaline.com/technology/corrosion-properties/</t>
   </si>
   <si>
-    <t>https://www.sii.co.jp/en/me/battery/products/silver-oxide/expiry-guide/#:~:text=The%20recommended%20usage%20period%20of,from%20the%20month%20of%20manufacturing.</t>
-  </si>
-  <si>
-    <t>https://galvanizeit.org/hot-dip-galvanizing/what-is-zinc/facts-about-zinc</t>
-  </si>
-  <si>
     <t>https://money.usnews.com/money/personal-finance/family-finance/articles/how-long-can-you-expect-your-roof-or-fridge-to-last#:~:text=Slate%2C%20copper%20and%20tile%20roofs,20%20years%2C%20the%20NAHB%20found.</t>
   </si>
   <si>
@@ -898,12 +892,6 @@
     <t>https://www.electronicsweekly.com/news/now-alternative-solid-tantalum-capacitors-2017-03/#:~:text=Whilst%20MLCCs%20are%20susceptible%20to,of%202%20years%20or%20less.</t>
   </si>
   <si>
-    <t>https://blog.epectec.com/understanding-how-solder-and-coatings-impact-pcb-shelf-life#:~:text=Depending%20on%20the%20solder%20that,last%20up%20to%2010%20years.</t>
-  </si>
-  <si>
-    <t>https://www.pv-magazine.com/2022/01/25/nickel-zinc-batteries-for-large-scale-backup-power/</t>
-  </si>
-  <si>
     <t>https://www.power-sonic.com/blog/features-of-sealed-lead-acid-batteries/#:~:text=Sealed%20lead%20acid%20batteries%20can,manufacturing%20process%20of%20the%20battery.</t>
   </si>
   <si>
@@ -913,12 +901,6 @@
     <t>https://digitalworld839.com/how-long-does-a-monitor-last/#:~:text=LCD%20monitors%20usually%20have%20a,for%20eight%20hours%20a%20day.</t>
   </si>
   <si>
-    <t>nuclear reactors :: https://www.energy.gov/ne/articles/whats-lifespan-nuclear-reactor-much-longer-you-might-think</t>
-  </si>
-  <si>
-    <t>https://crossroadsgalvanizing.com/2020/04/08/life-expectancy-of-galvanized-steel/</t>
-  </si>
-  <si>
     <t>solder /// https://www.evilmadscientist.com/2013/solder-expire/#:~:text=Flux%20cored%20solder%20wire%20has,years%20from%20date%20of%20manufacture.</t>
   </si>
   <si>
@@ -931,15 +913,9 @@
     <t>chemical ::: https://www.sciencedirect.com/science/article/pii/S0263436821000780</t>
   </si>
   <si>
-    <t>solar panels :: https://www.greenbiz.com/article/what-will-happen-solar-panels-after-their-useful-lives-are-over#:~:text=The%20industry%20standard%20life%20span,t%20long%20from%20being%20retired.</t>
-  </si>
-  <si>
     <t>https://blog.evbox.com/ev-battery-longevity#:~:text=How%20long%20do%20EV%20batteries,costs%20associated%20with%20battery%20replacement.</t>
   </si>
   <si>
-    <t>https://www.buildingenclosureonline.com/articles/88937-transit-centre-showcases-zinc-cladding-to-create-distinctive-durable-design</t>
-  </si>
-  <si>
     <t>https://www.heatandplumb.com/blog/how-often-should-radiators-be-replaced#:~:text=If%20you're%20asking%20%E2%80%9Chow,of%20how%20they're%20performing.</t>
   </si>
   <si>
@@ -1229,6 +1205,12 @@
   </si>
   <si>
     <t>Assuming half of silver jewelry can be directly remelted</t>
+  </si>
+  <si>
+    <t>assumed same as steel</t>
+  </si>
+  <si>
+    <t>assumed same as gold</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1315,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1351,18 +1333,6 @@
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1378,7 +1348,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1455,17 +1425,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -4366,7 +4331,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4444,7 +4409,7 @@
         <v>94</v>
       </c>
       <c r="Q1" s="36" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="R1" s="35" t="s">
         <v>95</v>
@@ -4504,7 +4469,7 @@
         <v>109</v>
       </c>
       <c r="AK1" s="35" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="14.5" customHeight="1">
@@ -4784,7 +4749,7 @@
         <v>133</v>
       </c>
       <c r="W5" s="9" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9"/>
@@ -4805,7 +4770,7 @@
         <v>220</v>
       </c>
       <c r="AF5" s="43" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="AG5" s="9" t="s">
         <v>221</v>
@@ -4900,23 +4865,23 @@
         <v>227</v>
       </c>
       <c r="AE6" s="7" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="AF6" s="7" t="s">
         <v>228</v>
       </c>
       <c r="AG6" s="42" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="AH6" s="7" t="s">
         <v>229</v>
       </c>
       <c r="AI6" s="43" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="AJ6" s="7"/>
       <c r="AK6" s="43" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:37" ht="14.5" customHeight="1">
@@ -4992,7 +4957,7 @@
         <v>230</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="AB7" s="9" t="s">
         <v>231</v>
@@ -5001,16 +4966,16 @@
         <v>78</v>
       </c>
       <c r="AD7" s="1" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="AE7" s="45" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="AF7" s="45" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AG7" s="45" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="AH7" s="9" t="s">
         <v>229</v>
@@ -5094,7 +5059,7 @@
         <v>234</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="AB8" s="7" t="s">
         <v>235</v>
@@ -5185,7 +5150,7 @@
         <v>238</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="AB9" s="9" t="s">
         <v>239</v>
@@ -5195,7 +5160,7 @@
       </c>
       <c r="AD9" s="9"/>
       <c r="AE9" s="9" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="AF9" s="9"/>
       <c r="AG9" s="9"/>
@@ -5246,7 +5211,7 @@
       <c r="M10" s="6">
         <v>0.15</v>
       </c>
-      <c r="N10" s="51">
+      <c r="N10" s="49">
         <f>1-N11-N9-N8-N7</f>
         <v>5.9998999999999955E-2</v>
       </c>
@@ -5282,7 +5247,7 @@
         <v>242</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="AB10" s="7" t="s">
         <v>243</v>
@@ -5373,7 +5338,7 @@
       <c r="Y11" s="9"/>
       <c r="Z11" s="9"/>
       <c r="AA11" s="1" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="AB11" s="9" t="s">
         <v>245</v>
@@ -5462,7 +5427,7 @@
       <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="AB12" s="7" t="s">
         <v>248</v>
@@ -5855,11 +5820,11 @@
       <c r="K17" s="8">
         <v>50</v>
       </c>
-      <c r="L17" s="46">
-        <v>30</v>
+      <c r="L17" s="8">
+        <v>50</v>
       </c>
       <c r="M17" s="8">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="N17" s="8">
         <v>50</v>
@@ -5902,22 +5867,22 @@
         <v>107</v>
       </c>
       <c r="AD17" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE17" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="AF17" s="9" t="s">
+        <v>373</v>
+      </c>
+      <c r="AG17" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="AF17" s="9" t="s">
+      <c r="AH17" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="AG17" s="9" t="s">
+      <c r="AI17" s="9" t="s">
         <v>264</v>
-      </c>
-      <c r="AH17" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="AI17" s="9" t="s">
-        <v>266</v>
       </c>
       <c r="AJ17" s="9"/>
       <c r="AK17" s="9"/>
@@ -5952,11 +5917,11 @@
       <c r="K18" s="6">
         <v>15</v>
       </c>
-      <c r="L18" s="52">
-        <v>1000000</v>
+      <c r="L18" s="6">
+        <v>3</v>
       </c>
       <c r="M18" s="6">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="N18" s="6">
         <v>5</v>
@@ -5989,32 +5954,32 @@
       <c r="X18" s="7"/>
       <c r="Y18" s="7"/>
       <c r="Z18" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="AA18" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="AB18" s="23" t="s">
         <v>267</v>
-      </c>
-      <c r="AA18" s="7" t="s">
-        <v>268</v>
-      </c>
-      <c r="AB18" s="23" t="s">
-        <v>269</v>
       </c>
       <c r="AC18" s="7" t="s">
         <v>107</v>
       </c>
       <c r="AD18" s="45" t="s">
-        <v>377</v>
-      </c>
-      <c r="AE18" s="7" t="s">
-        <v>270</v>
+        <v>369</v>
+      </c>
+      <c r="AE18" s="9" t="s">
+        <v>374</v>
       </c>
       <c r="AF18" s="7" t="s">
-        <v>271</v>
+        <v>373</v>
       </c>
       <c r="AG18" s="7"/>
       <c r="AH18" s="7" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="AI18" s="7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="AJ18" s="7"/>
       <c r="AK18" s="7"/>
@@ -6049,11 +6014,11 @@
       <c r="K19" s="8">
         <v>25</v>
       </c>
-      <c r="L19" s="46">
-        <v>3</v>
+      <c r="L19" s="8">
+        <v>30</v>
       </c>
       <c r="M19" s="8">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="N19" s="8">
         <v>20</v>
@@ -6092,22 +6057,22 @@
         <v>107</v>
       </c>
       <c r="AD19" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE19" s="9" t="s">
-        <v>275</v>
+        <v>374</v>
       </c>
       <c r="AF19" s="9" t="s">
-        <v>276</v>
+        <v>373</v>
       </c>
       <c r="AG19" s="9" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="AH19" s="9" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="AI19" s="24" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="AJ19" s="9"/>
       <c r="AK19" s="9"/>
@@ -6142,11 +6107,11 @@
       <c r="K20" s="6">
         <v>15</v>
       </c>
-      <c r="L20" s="47">
-        <v>80</v>
-      </c>
-      <c r="M20" s="15">
-        <v>1000000</v>
+      <c r="L20" s="6">
+        <v>15</v>
+      </c>
+      <c r="M20" s="6">
+        <v>15</v>
       </c>
       <c r="N20" s="6">
         <v>5</v>
@@ -6173,7 +6138,7 @@
       <c r="X20" s="7"/>
       <c r="Y20" s="7"/>
       <c r="Z20" s="7" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="AA20" s="7"/>
       <c r="AB20" s="7"/>
@@ -6181,14 +6146,16 @@
         <v>107</v>
       </c>
       <c r="AD20" s="45" t="s">
-        <v>377</v>
-      </c>
-      <c r="AE20" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="AF20" s="7"/>
+        <v>369</v>
+      </c>
+      <c r="AE20" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="AF20" s="7" t="s">
+        <v>373</v>
+      </c>
       <c r="AG20" s="7" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
@@ -6226,10 +6193,10 @@
         <v>22</v>
       </c>
       <c r="L21" s="8">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="M21" s="8">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="N21" s="8">
         <v>17</v>
@@ -6263,26 +6230,28 @@
       <c r="Y21" s="9"/>
       <c r="Z21" s="9"/>
       <c r="AA21" s="9" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="AC21" s="9" t="s">
         <v>107</v>
       </c>
       <c r="AD21" s="45" t="s">
-        <v>377</v>
-      </c>
-      <c r="AE21" s="9"/>
+        <v>369</v>
+      </c>
+      <c r="AE21" s="9" t="s">
+        <v>374</v>
+      </c>
       <c r="AF21" s="9" t="s">
-        <v>283</v>
+        <v>373</v>
       </c>
       <c r="AG21" s="9" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="AH21" s="9" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="AI21" s="9" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="9"/>
@@ -6344,23 +6313,23 @@
       <c r="X22" s="7"/>
       <c r="Z22" s="9"/>
       <c r="AA22" s="45" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="AB22" s="6"/>
       <c r="AC22" s="7" t="s">
         <v>183</v>
       </c>
       <c r="AD22" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE22" s="7" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="AF22" s="42" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AG22" s="7" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="AH22" s="7"/>
       <c r="AI22" s="7"/>
@@ -6424,23 +6393,23 @@
       <c r="X23" s="9"/>
       <c r="Z23" s="7"/>
       <c r="AA23" s="45" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9" t="s">
         <v>183</v>
       </c>
       <c r="AD23" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE23" s="7" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="AF23" s="42" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AG23" s="7" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="AH23" s="9"/>
       <c r="AI23" s="9"/>
@@ -6504,23 +6473,23 @@
       <c r="X24" s="7"/>
       <c r="Z24" s="9"/>
       <c r="AA24" s="45" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="AB24" s="6"/>
       <c r="AC24" s="7" t="s">
         <v>183</v>
       </c>
       <c r="AD24" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE24" s="7" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="AF24" s="42" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AG24" s="7" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="AH24" s="7"/>
       <c r="AI24" s="7"/>
@@ -6584,23 +6553,23 @@
       <c r="X25" s="9"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="45" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="AB25" s="8"/>
       <c r="AC25" s="9" t="s">
         <v>183</v>
       </c>
       <c r="AD25" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE25" s="7" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="AF25" s="42" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AG25" s="7" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="AH25" s="9"/>
       <c r="AI25" s="9"/>
@@ -6665,23 +6634,23 @@
       <c r="Y26" s="8"/>
       <c r="Z26" s="9"/>
       <c r="AA26" s="45" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="AB26" s="8"/>
       <c r="AC26" s="7" t="s">
         <v>183</v>
       </c>
       <c r="AD26" s="45" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="AE26" s="7" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="AF26" s="42" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="AG26" s="1" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="AH26" s="7"/>
       <c r="AI26" s="7"/>
@@ -6755,23 +6724,23 @@
       <c r="X27" s="9"/>
       <c r="Y27" s="9"/>
       <c r="Z27" s="21" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="AA27" s="9"/>
       <c r="AB27" s="21" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AC27" s="9" t="s">
         <v>77</v>
       </c>
       <c r="AD27" s="9"/>
       <c r="AE27" s="9" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="AF27" s="9"/>
       <c r="AG27" s="9"/>
       <c r="AH27" s="9" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="AI27" s="9"/>
       <c r="AJ27" s="9"/>
@@ -6842,25 +6811,25 @@
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="AA28" s="7"/>
       <c r="AB28" s="23" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="AC28" s="7" t="s">
         <v>77</v>
       </c>
       <c r="AD28" s="7"/>
       <c r="AE28" s="7" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="AF28" s="7" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="AG28" s="7"/>
       <c r="AH28" s="7" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="AI28" s="7"/>
       <c r="AJ28" s="7"/>
@@ -7010,7 +6979,7 @@
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
       <c r="Z30" s="23" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="AA30" s="7"/>
       <c r="AB30" s="7"/>
@@ -7018,13 +6987,13 @@
         <v>77</v>
       </c>
       <c r="AD30" s="7" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="AE30" s="7"/>
       <c r="AF30" s="7"/>
       <c r="AG30" s="7"/>
       <c r="AH30" s="29" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="AI30" s="7"/>
       <c r="AJ30" s="7"/>
@@ -7090,7 +7059,7 @@
         <v>131</v>
       </c>
       <c r="W31" s="9" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="X31" s="9"/>
       <c r="Y31" s="9"/>
@@ -7102,7 +7071,7 @@
       </c>
       <c r="AD31" s="9"/>
       <c r="AE31" s="9" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="AF31" s="9"/>
       <c r="AG31" s="9"/>
@@ -7171,7 +7140,7 @@
         <v>131</v>
       </c>
       <c r="W32" s="9" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
@@ -7183,7 +7152,7 @@
       </c>
       <c r="AD32" s="7"/>
       <c r="AE32" s="9" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="AF32" s="7"/>
       <c r="AG32" s="7"/>
@@ -7257,24 +7226,24 @@
       <c r="Z33" s="9"/>
       <c r="AA33" s="9"/>
       <c r="AB33" s="9" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="AC33" s="9" t="s">
         <v>77</v>
       </c>
       <c r="AD33" s="9" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="AE33" s="9"/>
       <c r="AF33" s="9"/>
       <c r="AG33" s="9"/>
       <c r="AH33" s="21" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="AI33" s="9"/>
       <c r="AJ33" s="9"/>
       <c r="AK33" s="9" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:37" ht="14.5" customHeight="1">
@@ -7344,11 +7313,11 @@
         <v>77</v>
       </c>
       <c r="AD34" s="23" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="AE34" s="7"/>
       <c r="AF34" s="7" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="AG34" s="7"/>
       <c r="AH34" s="7"/>
@@ -7422,13 +7391,13 @@
       <c r="X35" s="9"/>
       <c r="Y35" s="9"/>
       <c r="Z35" s="9" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="AA35" s="9" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="AB35" s="9" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="AC35" s="9" t="s">
         <v>91</v>
@@ -7436,7 +7405,7 @@
       <c r="AD35" s="9"/>
       <c r="AE35" s="9"/>
       <c r="AF35" s="9" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="AG35" s="9"/>
       <c r="AH35" s="9" t="s">
@@ -7448,7 +7417,7 @@
     </row>
     <row r="36" spans="1:37" ht="14.5" customHeight="1">
       <c r="A36" s="6" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B36" s="6">
         <v>0.5</v>
@@ -7517,7 +7486,7 @@
       <c r="AF36" s="6"/>
       <c r="AG36" s="6"/>
       <c r="AH36" s="6" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="AI36" s="6"/>
       <c r="AJ36" s="6"/>
@@ -7588,10 +7557,10 @@
       </c>
       <c r="Y37" s="9"/>
       <c r="Z37" s="9" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="AA37" s="21" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="AB37" s="9" t="s">
         <v>208</v>
@@ -7603,7 +7572,7 @@
       <c r="AG37" s="9"/>
       <c r="AH37" s="9"/>
       <c r="AI37" s="9" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="AJ37" s="9"/>
       <c r="AK37" s="9"/>
@@ -7903,10 +7872,10 @@
         <v>34</v>
       </c>
       <c r="T41" s="9" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="U41" s="9" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="V41" s="9" t="s">
         <v>89</v>
@@ -8009,28 +7978,28 @@
       <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
       <c r="Z42" s="23" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="AA42" s="7"/>
       <c r="AB42" s="23" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="AC42" s="7" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="AD42" s="7"/>
       <c r="AE42" s="43" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="AF42" s="7"/>
       <c r="AG42" s="23" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="AH42" s="7"/>
       <c r="AI42" s="7"/>
       <c r="AJ42" s="7"/>
       <c r="AK42" s="7" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="43" spans="1:37" ht="14.5" customHeight="1">
@@ -8101,22 +8070,22 @@
       </c>
       <c r="Y43" s="8"/>
       <c r="Z43" s="24" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="AA43" s="8" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="AB43" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="AC43" s="8" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="AD43" s="8" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="AE43" s="8" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="AF43" s="8" t="s">
         <v>172</v>
@@ -8194,7 +8163,7 @@
       <c r="X44" s="7"/>
       <c r="Y44" s="7"/>
       <c r="Z44" s="7" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="AA44" s="7"/>
       <c r="AB44" s="7"/>
@@ -8285,7 +8254,7 @@
       <c r="X45" s="9"/>
       <c r="Y45" s="9"/>
       <c r="Z45" s="9" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="AA45" s="9"/>
       <c r="AB45" s="9"/>
@@ -9658,47 +9627,47 @@
       <c r="AK73" s="9"/>
     </row>
     <row r="74" spans="1:37">
-      <c r="A74" s="48" t="s">
+      <c r="A74" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B74" s="48"/>
-      <c r="C74" s="48"/>
-      <c r="D74" s="48"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="48"/>
-      <c r="H74" s="48"/>
-      <c r="I74" s="48"/>
-      <c r="J74" s="48"/>
-      <c r="K74" s="48"/>
-      <c r="L74" s="48"/>
-      <c r="M74" s="48"/>
-      <c r="N74" s="48"/>
-      <c r="O74" s="48"/>
-      <c r="P74" s="48"/>
-      <c r="Q74" s="49"/>
-      <c r="R74" s="48"/>
-      <c r="S74" s="48" t="s">
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="46"/>
+      <c r="I74" s="46"/>
+      <c r="J74" s="46"/>
+      <c r="K74" s="46"/>
+      <c r="L74" s="46"/>
+      <c r="M74" s="46"/>
+      <c r="N74" s="46"/>
+      <c r="O74" s="46"/>
+      <c r="P74" s="46"/>
+      <c r="Q74" s="47"/>
+      <c r="R74" s="46"/>
+      <c r="S74" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="T74" s="50"/>
-      <c r="U74" s="50"/>
-      <c r="V74" s="50"/>
-      <c r="W74" s="50"/>
-      <c r="X74" s="50"/>
-      <c r="Y74" s="50"/>
-      <c r="Z74" s="50"/>
-      <c r="AA74" s="50"/>
-      <c r="AB74" s="50"/>
-      <c r="AC74" s="50"/>
-      <c r="AD74" s="50"/>
-      <c r="AE74" s="50"/>
-      <c r="AF74" s="50"/>
-      <c r="AG74" s="50"/>
-      <c r="AH74" s="50"/>
-      <c r="AI74" s="50"/>
-      <c r="AJ74" s="50"/>
-      <c r="AK74" s="50"/>
+      <c r="T74" s="48"/>
+      <c r="U74" s="48"/>
+      <c r="V74" s="48"/>
+      <c r="W74" s="48"/>
+      <c r="X74" s="48"/>
+      <c r="Y74" s="48"/>
+      <c r="Z74" s="48"/>
+      <c r="AA74" s="48"/>
+      <c r="AB74" s="48"/>
+      <c r="AC74" s="48"/>
+      <c r="AD74" s="48"/>
+      <c r="AE74" s="48"/>
+      <c r="AF74" s="48"/>
+      <c r="AG74" s="48"/>
+      <c r="AH74" s="48"/>
+      <c r="AI74" s="48"/>
+      <c r="AJ74" s="48"/>
+      <c r="AK74" s="48"/>
     </row>
     <row r="90" spans="1:30">
       <c r="A90" s="8" t="s">
@@ -9709,25 +9678,25 @@
         <v>0.19100000000000006</v>
       </c>
       <c r="F90" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G90" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="H90" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="AA90" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="AB90" t="s">
         <v>236</v>
       </c>
       <c r="AC90" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="AD90" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="91" spans="1:30">
@@ -9769,22 +9738,22 @@
         <v>0.24149999999999999</v>
       </c>
       <c r="F92" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="G92" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="H92" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="AA92" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="AB92" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="AC92" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="93" spans="1:30">
@@ -9901,10 +9870,10 @@
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E2" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -10305,10 +10274,10 @@
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -10386,7 +10355,7 @@
         <v>12543.399838585501</v>
       </c>
       <c r="C9" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="E9" s="41">
         <v>3592.3557497575903</v>
@@ -10583,19 +10552,19 @@
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E2" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="H2" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="I2" t="s">
         <v>191</v>
       </c>
       <c r="J2" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -12609,7 +12578,7 @@
         <v>199</v>
       </c>
       <c r="H1" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="L1" t="s">
         <v>188</v>
@@ -12618,7 +12587,7 @@
         <v>188</v>
       </c>
       <c r="Q1" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -12626,29 +12595,29 @@
         <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="C2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>201</v>
       </c>
       <c r="E2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="H2" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="L2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="M2" s="39"/>
       <c r="Q2" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -13490,7 +13459,7 @@
         <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -14235,13 +14204,13 @@
         <v>176</v>
       </c>
       <c r="B2" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="D2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">
@@ -15073,11 +15042,11 @@
         <v>176</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16">

</xml_diff>